<commit_message>
Added Chatbox class.(semi-complete) Now player needs to verify if there really is a scam in the ChatRoom. Difficulty is now tracked by an int.
</commit_message>
<xml_diff>
--- a/List of Tasks.xlsx
+++ b/List of Tasks.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MrAnoimus\Desktop\School Work\Year 2\Sem 2\Mobile Game Development\Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mr. Fatal\Desktop\School Work\Mobile\Android Dev\why-are-we-doing-this-productions-first-game\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Yu Xuan</t>
   </si>
@@ -41,24 +41,15 @@
     <t>onTouch Events(Buttons to pages)</t>
   </si>
   <si>
-    <t>Sliders</t>
-  </si>
-  <si>
     <t>RNG(Chances of a room out of the 4 to have a scammer)</t>
   </si>
   <si>
     <t>Art Assets</t>
   </si>
   <si>
-    <t>Created an array of chatrooms</t>
-  </si>
-  <si>
     <t>Layout of pages</t>
   </si>
   <si>
-    <t>Enhanced touch detection for rooms, only red rooms can be touch to score</t>
-  </si>
-  <si>
     <t>Scores(Minus score if leave chatrooms be if red after sometime, touch wrong door)</t>
   </si>
   <si>
@@ -74,7 +65,13 @@
     <t xml:space="preserve"> touch with rooms</t>
   </si>
   <si>
-    <t>Toggles (Easy mode or hard mode, not working now)</t>
+    <t>Chatroom class</t>
+  </si>
+  <si>
+    <t>Enhanced touch detection for rooms, only red rooms can be touched to score</t>
+  </si>
+  <si>
+    <t>Options menu (Sliders, toggles)</t>
   </si>
 </sst>
 </file>
@@ -122,19 +119,21 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -145,14 +144,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,13 +436,13 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="74.42578125" customWidth="1"/>
-    <col min="3" max="3" width="66.7109375" customWidth="1"/>
+    <col min="3" max="3" width="70.28515625" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -475,7 +475,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -494,7 +494,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -507,10 +507,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -523,10 +523,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -539,10 +539,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -554,11 +554,11 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -567,10 +567,10 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1"/>
@@ -581,17 +581,10 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
+      <c r="A11" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>